<commit_message>
download files from drive
</commit_message>
<xml_diff>
--- a/files/New DailyRewards.xlsx
+++ b/files/New DailyRewards.xlsx
@@ -128,7 +128,7 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
@@ -374,8 +374,8 @@
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3">
-        <v>15.0</v>
+      <c r="C2" s="4">
+        <v>5.0</v>
       </c>
     </row>
     <row r="3">
@@ -416,10 +416,10 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="3">
-        <v>200.0</v>
+        <v>3</v>
+      </c>
+      <c r="C6" s="4">
+        <v>10.0</v>
       </c>
     </row>
     <row r="7">

</xml_diff>